<commit_message>
added records for tables and their corresponding websites in spreadsheet
</commit_message>
<xml_diff>
--- a/src/scraping/table names per site.xlsx
+++ b/src/scraping/table names per site.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="184">
   <si>
     <t xml:space="preserve">Table Name</t>
   </si>
@@ -34,24 +34,36 @@
     <t xml:space="preserve">https://mobilendloan.com/</t>
   </si>
   <si>
+    <t xml:space="preserve">limit hit for https://mobileendloan.com above 700k (format HA0000002)</t>
+  </si>
+  <si>
     <t xml:space="preserve">scraper2_info</t>
   </si>
   <si>
     <t xml:space="preserve">https://myonlineloanpro.com/</t>
   </si>
   <si>
+    <t xml:space="preserve">able to scrape up to 280k until IP banned for https://myonlineloanpro.com. The proxy was introduced. Was able to scrape shortly until they implement rate limit. Changing headers and proxy seem to not work</t>
+  </si>
+  <si>
     <t xml:space="preserve">scraper3_info</t>
   </si>
   <si>
     <t xml:space="preserve">https://xmydebt.com</t>
   </si>
   <si>
+    <t xml:space="preserve">on queue</t>
+  </si>
+  <si>
     <t xml:space="preserve">scraper4_info</t>
   </si>
   <si>
     <t xml:space="preserve">https://moneyladdernow.com</t>
   </si>
   <si>
+    <t xml:space="preserve">done scraping using common names. Scraping again using updated names as of 12/8</t>
+  </si>
+  <si>
     <t xml:space="preserve">scraper5_info</t>
   </si>
   <si>
@@ -70,6 +82,9 @@
     <t xml:space="preserve">https://24hrwire.com</t>
   </si>
   <si>
+    <t xml:space="preserve">done scraping using common names. On queue for scraping using updated names.</t>
+  </si>
+  <si>
     <t xml:space="preserve">scraper8_info</t>
   </si>
   <si>
@@ -130,6 +145,9 @@
     <t xml:space="preserve">https://callrvf.com</t>
   </si>
   <si>
+    <t xml:space="preserve">scraping in progress</t>
+  </si>
+  <si>
     <t xml:space="preserve">scraper18_info</t>
   </si>
   <si>
@@ -206,6 +224,354 @@
   </si>
   <si>
     <t xml:space="preserve">https://getmyadv.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper31_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://getmyadvloan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper32_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://getnsc.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper33_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://getrfsnow.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper34_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://goadvloan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper35_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://goadvtoday.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper36_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gonewstart.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper37_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gowithadv.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper38_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gowithunited.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper39_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://grtdebt.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper40_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://letstryadv.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper41_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://myadvanloan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper42_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bhgelite.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraping in progress - priority HIGH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper43_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://myadvloans.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper44_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://myadvnow.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper45_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://myadvtoday.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper46_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mygwcloan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper47_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mysigloan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper48_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://newchaptergo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper49_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nsftoday.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper50_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ptrdebt.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper51_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://rchlend.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper52_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://rmftoday.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper53_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://safestonenow.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper54_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sigloan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper55_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://topadvloan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper56_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tryadv.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper57_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tryadvan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper58_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tryadvloan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper59_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tryadvnow.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper60_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tryadvtoday.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper61_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tryaflnow.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper62_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tryatlasds.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper63_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tryavantoday.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper64_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://trybpfnow.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper65_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://trycoa.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper66_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://trycwdnow.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper67_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://trycwf.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper68_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://trymyadv.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper69_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://trynavnow.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper70_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tryodycg.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper71_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://trysecone.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper72_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://trysncnow.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper73_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tryttn.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper74_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youradvan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper75_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youradvloan.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper76_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper77_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper78_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper79_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper80_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper81_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper82_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper83_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper84_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper85_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper86_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper87_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper88_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper89_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper90_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper91_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper92_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper93_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper94_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper95_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper96_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper97_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper98_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper99_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scraper100_info</t>
   </si>
 </sst>
 </file>
@@ -220,6 +586,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -241,6 +608,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -311,16 +679,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -338,271 +708,929 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://mobilendloan.com/"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://myonlineloanpro.com/"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://xmydebt.com"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://moneyladdernow.com"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://mylibertyone.com"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://advtrelief.com"/>
-    <hyperlink ref="B8" r:id="rId7" display="https://24hrwire.com"/>
-    <hyperlink ref="B9" r:id="rId8" display="https://advdebt.com"/>
-    <hyperlink ref="B10" r:id="rId9" display="https://advdebthelp.com"/>
-    <hyperlink ref="B11" r:id="rId10" display="https://advpref.com"/>
-    <hyperlink ref="B12" r:id="rId11" display="https://advprefer.com"/>
-    <hyperlink ref="B13" r:id="rId12" display="https://advrelief.com"/>
-    <hyperlink ref="B14" r:id="rId13" display="https://advworks4u.com"/>
-    <hyperlink ref="B15" r:id="rId14" display="https://calladvloan.com"/>
-    <hyperlink ref="B16" r:id="rId15" display="https://calladvnow.com"/>
-    <hyperlink ref="B17" r:id="rId16" display="https://calladvtoday.com"/>
-    <hyperlink ref="B18" r:id="rId17" display="https://callrvf.com"/>
-    <hyperlink ref="B19" r:id="rId18" display="https://chooseadv.com"/>
-    <hyperlink ref="B20" r:id="rId19" display="https://getadgnow.com"/>
-    <hyperlink ref="B21" r:id="rId20" display="https://getadvloan.com"/>
-    <hyperlink ref="B22" r:id="rId21" display="https://getadvnow.com"/>
-    <hyperlink ref="B23" r:id="rId22" display="https://getadvrelief.com"/>
-    <hyperlink ref="B24" r:id="rId23" display="https://getadvtoday.com"/>
-    <hyperlink ref="B25" r:id="rId24" display="https://getbenefit1st.com"/>
-    <hyperlink ref="B26" r:id="rId25" display="https://getbtf.com"/>
-    <hyperlink ref="B27" r:id="rId26" display="https://getcen.com"/>
-    <hyperlink ref="B28" r:id="rId27" display="https://getfcfnow.com"/>
-    <hyperlink ref="B29" r:id="rId28" display="https://getgwf.com"/>
-    <hyperlink ref="B30" r:id="rId29" display="https://getidsnow.com"/>
-    <hyperlink ref="B31" r:id="rId30" display="https://getmyadv.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="limit hit for https://mobileendloan.com above 700k (format HA0000002)"/>
+    <hyperlink ref="B3" r:id="rId3" display="https://myonlineloanpro.com/"/>
+    <hyperlink ref="C3" r:id="rId4" display="able to scrape up to 280k until IP banned for https://myonlineloanpro.com. The proxy was introduced. Was able to scrape shortly until they implement rate limit. Changing headers and proxy seem to not work"/>
+    <hyperlink ref="B4" r:id="rId5" display="https://xmydebt.com"/>
+    <hyperlink ref="B5" r:id="rId6" display="https://moneyladdernow.com"/>
+    <hyperlink ref="B6" r:id="rId7" display="https://mylibertyone.com"/>
+    <hyperlink ref="B7" r:id="rId8" display="https://advtrelief.com"/>
+    <hyperlink ref="B8" r:id="rId9" display="https://24hrwire.com"/>
+    <hyperlink ref="B9" r:id="rId10" display="https://advdebt.com"/>
+    <hyperlink ref="B10" r:id="rId11" display="https://advdebthelp.com"/>
+    <hyperlink ref="B11" r:id="rId12" display="https://advpref.com"/>
+    <hyperlink ref="B12" r:id="rId13" display="https://advprefer.com"/>
+    <hyperlink ref="B13" r:id="rId14" display="https://advrelief.com"/>
+    <hyperlink ref="B14" r:id="rId15" display="https://advworks4u.com"/>
+    <hyperlink ref="B15" r:id="rId16" display="https://calladvloan.com"/>
+    <hyperlink ref="B16" r:id="rId17" display="https://calladvnow.com"/>
+    <hyperlink ref="B17" r:id="rId18" display="https://calladvtoday.com"/>
+    <hyperlink ref="B18" r:id="rId19" display="https://callrvf.com"/>
+    <hyperlink ref="B19" r:id="rId20" display="https://chooseadv.com"/>
+    <hyperlink ref="B20" r:id="rId21" display="https://getadgnow.com"/>
+    <hyperlink ref="B21" r:id="rId22" display="https://getadvloan.com"/>
+    <hyperlink ref="B22" r:id="rId23" display="https://getadvnow.com"/>
+    <hyperlink ref="B23" r:id="rId24" display="https://getadvrelief.com"/>
+    <hyperlink ref="B24" r:id="rId25" display="https://getadvtoday.com"/>
+    <hyperlink ref="B25" r:id="rId26" display="https://getbenefit1st.com"/>
+    <hyperlink ref="B26" r:id="rId27" display="https://getbtf.com"/>
+    <hyperlink ref="B27" r:id="rId28" display="https://getcen.com"/>
+    <hyperlink ref="B28" r:id="rId29" display="https://getfcfnow.com"/>
+    <hyperlink ref="B29" r:id="rId30" display="https://getgwf.com"/>
+    <hyperlink ref="B30" r:id="rId31" display="https://getidsnow.com"/>
+    <hyperlink ref="B31" r:id="rId32" display="https://getmyadv.com"/>
+    <hyperlink ref="B32" r:id="rId33" display="https://getmyadvloan.com"/>
+    <hyperlink ref="B33" r:id="rId34" display="https://getnsc.com"/>
+    <hyperlink ref="B34" r:id="rId35" display="https://getrfsnow.com"/>
+    <hyperlink ref="B35" r:id="rId36" display="https://goadvloan.com"/>
+    <hyperlink ref="B36" r:id="rId37" display="https://goadvtoday.com"/>
+    <hyperlink ref="B37" r:id="rId38" display="https://gonewstart.com"/>
+    <hyperlink ref="B38" r:id="rId39" display="https://gowithadv.com"/>
+    <hyperlink ref="B39" r:id="rId40" display="https://gowithunited.com"/>
+    <hyperlink ref="B40" r:id="rId41" display="https://grtdebt.com"/>
+    <hyperlink ref="B41" r:id="rId42" display="https://letstryadv.com"/>
+    <hyperlink ref="B42" r:id="rId43" display="https://myadvanloan.com"/>
+    <hyperlink ref="B43" r:id="rId44" display="https://bhgelite.com"/>
+    <hyperlink ref="B44" r:id="rId45" display="https://myadvloans.com"/>
+    <hyperlink ref="B45" r:id="rId46" display="https://myadvnow.com"/>
+    <hyperlink ref="B46" r:id="rId47" display="https://myadvtoday.com"/>
+    <hyperlink ref="B47" r:id="rId48" display="https://mygwcloan.com"/>
+    <hyperlink ref="B48" r:id="rId49" display="https://mysigloan.com"/>
+    <hyperlink ref="B49" r:id="rId50" display="https://newchaptergo.com"/>
+    <hyperlink ref="B50" r:id="rId51" display="https://nsftoday.com"/>
+    <hyperlink ref="B51" r:id="rId52" display="https://ptrdebt.com"/>
+    <hyperlink ref="B52" r:id="rId53" display="https://rchlend.com"/>
+    <hyperlink ref="B53" r:id="rId54" display="https://rmftoday.com"/>
+    <hyperlink ref="B54" r:id="rId55" display="https://safestonenow.com"/>
+    <hyperlink ref="B55" r:id="rId56" display="https://sigloan.com"/>
+    <hyperlink ref="B56" r:id="rId57" display="https://topadvloan.com"/>
+    <hyperlink ref="B57" r:id="rId58" display="https://tryadv.com"/>
+    <hyperlink ref="B58" r:id="rId59" display="https://tryadvan.com"/>
+    <hyperlink ref="B59" r:id="rId60" display="https://tryadvloan.com"/>
+    <hyperlink ref="B60" r:id="rId61" display="https://tryadvnow.com"/>
+    <hyperlink ref="B61" r:id="rId62" display="https://tryadvtoday.com"/>
+    <hyperlink ref="B62" r:id="rId63" display="https://tryaflnow.com"/>
+    <hyperlink ref="B63" r:id="rId64" display="https://tryatlasds.com"/>
+    <hyperlink ref="B64" r:id="rId65" display="https://tryavantoday.com"/>
+    <hyperlink ref="B65" r:id="rId66" display="https://trybpfnow.com"/>
+    <hyperlink ref="B66" r:id="rId67" display="https://trycoa.com"/>
+    <hyperlink ref="B67" r:id="rId68" display="https://trycwdnow.com"/>
+    <hyperlink ref="B68" r:id="rId69" display="https://trycwf.com"/>
+    <hyperlink ref="B69" r:id="rId70" display="https://trymyadv.com"/>
+    <hyperlink ref="B70" r:id="rId71" display="https://trynavnow.com"/>
+    <hyperlink ref="B71" r:id="rId72" display="https://tryodycg.com"/>
+    <hyperlink ref="B72" r:id="rId73" display="https://trysecone.com"/>
+    <hyperlink ref="B73" r:id="rId74" display="https://trysncnow.com"/>
+    <hyperlink ref="B74" r:id="rId75" display="https://tryttn.com"/>
+    <hyperlink ref="B75" r:id="rId76" display="https://youradvan.com"/>
+    <hyperlink ref="B76" r:id="rId77" display="https://youradvloan.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>